<commit_message>
Finished BOM and purchasing
</commit_message>
<xml_diff>
--- a/RemoteLabs_supervisor_PCB/BOM_SUPERVISOR_REMOTELABS_INITIAL.xlsx
+++ b/RemoteLabs_supervisor_PCB/BOM_SUPERVISOR_REMOTELABS_INITIAL.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="351">
   <si>
     <t>Ref</t>
   </si>
@@ -201,9 +201,6 @@
     <t>USB_A</t>
   </si>
   <si>
-    <t>USB_A_1</t>
-  </si>
-  <si>
     <t>Connector_USB:USB_A_Molex_67643_Horizontal</t>
   </si>
   <si>
@@ -249,18 +246,12 @@
     <t>Conn_01x03_Male</t>
   </si>
   <si>
-    <t>Screw_Terminal_01x02</t>
-  </si>
-  <si>
     <t>TerminalBlock:TerminalBlock_Altech_AK300-2_P5.00mm</t>
   </si>
   <si>
     <t>Generic screw terminal, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
-    <t>Screw_Terminal_01x03</t>
-  </si>
-  <si>
     <t>TerminalBlock:TerminalBlock_Altech_AK300-3_P5.00mm</t>
   </si>
   <si>
@@ -339,9 +330,6 @@
     <t>2k2</t>
   </si>
   <si>
-    <t>Resistor_0805</t>
-  </si>
-  <si>
     <t>Resistor_SMD:R_0805_2012Metric_Pad1.20x1.40mm_HandSolder</t>
   </si>
   <si>
@@ -384,9 +372,6 @@
     <t>Stepper_Mode</t>
   </si>
   <si>
-    <t>SW_DIP_x03</t>
-  </si>
-  <si>
     <t>Button_Switch_SMD:SW_DIP_SPSTx03_Slide_6.7x9.18mm_W6.73mm_P2.54mm_LowProfile_JPin</t>
   </si>
   <si>
@@ -438,9 +423,6 @@
     <t xml:space="preserve">U8, </t>
   </si>
   <si>
-    <t>4069_3</t>
-  </si>
-  <si>
     <t>Package_DIP:SMDIP-14_W9.53mm</t>
   </si>
   <si>
@@ -450,9 +432,6 @@
     <t xml:space="preserve">U9, U10, U11, U12, </t>
   </si>
   <si>
-    <t>4081_5</t>
-  </si>
-  <si>
     <t>Quad And 2 inputs</t>
   </si>
   <si>
@@ -462,9 +441,6 @@
     <t>74HC86</t>
   </si>
   <si>
-    <t>74HC86_9</t>
-  </si>
-  <si>
     <t>Quad 2-input XOR</t>
   </si>
   <si>
@@ -639,9 +615,6 @@
     <t>ReplaCED WITH Ferrite as per Arduino Nano IoT</t>
   </si>
   <si>
-    <t>pushbutton_tactile_2pin_SMD</t>
-  </si>
-  <si>
     <t>MEC 5E single pole normally-open tactile switch</t>
   </si>
   <si>
@@ -708,9 +681,6 @@
     <t>55 in stock</t>
   </si>
   <si>
-    <t>https://uk.farnell.com/avx/08055c104k4z2a/cap-0-1-f-50v-10-x7r-0805/dp/1301717?st=100n%200805</t>
-  </si>
-  <si>
     <t>https://uk.farnell.com/kemet/edk107m035a9haa/cap-100-f-35v-radial-smd-reel/dp/2068675?st=100uf</t>
   </si>
   <si>
@@ -1009,6 +979,99 @@
   </si>
   <si>
     <t>Fuseholder, Open Design, 250V, 10A, 5 x 20mm, Through Hole, Black</t>
+  </si>
+  <si>
+    <t>Pin Header, Square Pin, Signal, Wire-to-Board, 2.54 mm, 1 Rows, 5 Contacts, Through Hole Straight</t>
+  </si>
+  <si>
+    <t>Pin Header, Straight, Board-to-Board, 2.54 mm, 1 Rows, 3 Contacts, Through Hole, M20</t>
+  </si>
+  <si>
+    <t>Pin Header, Board-to-Board, 2.54 mm, 1 Rows, 20 Contacts, Through Hole, M20</t>
+  </si>
+  <si>
+    <t>PCB Receptacle, Board-to-Board, 2.54 mm, 1 Rows, 20 Contacts, Through Hole Mount, 2212S</t>
+  </si>
+  <si>
+    <t>USB Stacked Connector, USB Type A, USB 2.0, 4 Ways, Right Angle, Brass, Gold Plated Contacts</t>
+  </si>
+  <si>
+    <t>USB Connector, Mini USB Type B, USB 2.0, Receptacle, 5 Ways, Surface Mount, Right Angle</t>
+  </si>
+  <si>
+    <t>Wire-To-Board Terminal Block, 5.08 mm, 2 Ways, 26 AWG, 12 AWG, Screw</t>
+  </si>
+  <si>
+    <t>Wire-To-Board Terminal Block, 5.08 mm, 3 Ways, 26 AWG, 12 AWG, Screw</t>
+  </si>
+  <si>
+    <t>Pin Header, Signal, Wire-to-Board, 2.54 mm, 1 Rows, 2 Contacts, Through Hole Straight, KK 254 6373</t>
+  </si>
+  <si>
+    <t>Pin Header, Signal, Wire-to-Board, 2.54 mm, 1 Rows, 3 Contacts, Through Hole Straight, KK 254 6373</t>
+  </si>
+  <si>
+    <t>Power MOSFET, P Channel, 55 V, 31 A, 0.06 ohm, TO-220AB, Through Hole</t>
+  </si>
+  <si>
+    <t>SMD Chip Resistor, 2.2 kohm, ± 1%, 250 mW, 0805 [2012 Metric], Thick Film, High Power</t>
+  </si>
+  <si>
+    <t>SMD Chip Resistor, 330 ohm, ± 1%, 250 mW, 0805 [2012 Metric], Thick Film, High Power</t>
+  </si>
+  <si>
+    <t>SMD Chip Resistor, 1 Mohm, ± 1%, 125 mW, 0805 [2012 Metric], Thick Film, General Purpose</t>
+  </si>
+  <si>
+    <t>SMD Chip Resistor, 1 kohm, ± 1%, 333.3 mW, 0805 [2012 Metric], Thick Film, General Purpose</t>
+  </si>
+  <si>
+    <t>SMD Chip Resistor, 470 ohm, ± 1%, 250 mW, 0805 [2012 Metric], Thick Film, High Power</t>
+  </si>
+  <si>
+    <t>SMD Chip Resistor, 10 kohm, ± 1%, 125 mW, 0805 [2012 Metric], Thick Film, General Purpose</t>
+  </si>
+  <si>
+    <t>2447553RL</t>
+  </si>
+  <si>
+    <t>SMD Chip Resistor, 2.7 kohm, ± 1%, 125 mW, 0805 [2012 Metric], Thick Film, General Purpose</t>
+  </si>
+  <si>
+    <t>DIP / SIP Switch, 3 Circuits, Flush Slide, Surface Mount, SPST, 50 V, 100 mA</t>
+  </si>
+  <si>
+    <t>Tactile Switch, PT645, Top Actuated, Surface Mount, Round Button, 160 gf, 50mA at 12VDC</t>
+  </si>
+  <si>
+    <t>2320087RL</t>
+  </si>
+  <si>
+    <t>Fixed LDO Voltage Regulator, 3.5V to 20V, 1.07V Dropout, 3.3Vout, 1Aout, SOT-223-3</t>
+  </si>
+  <si>
+    <t>1652366RL</t>
+  </si>
+  <si>
+    <t>Shift Register, HEF4094, 1 Element, 8 bit, SOIC, 16 Pins</t>
+  </si>
+  <si>
+    <t>Logic IC, Inverter, Hex, 1 Inputs, 14 Pins, SOIC, 4069</t>
+  </si>
+  <si>
+    <t>Logic IC, AND Gate, Quad, 2 Inputs, 14 Pins, SOIC, 4081</t>
+  </si>
+  <si>
+    <t>Logic IC, XOR (Exclusive OR), Quad, 2 Inputs, 14 Pins, SOIC, 74HC86</t>
+  </si>
+  <si>
+    <t>Operational Amplifier, Rail-to-Rail O/P, 4 Amplifier, 3 MHz, 2.8 V/µs</t>
+  </si>
+  <si>
+    <t>Accounted For Below</t>
+  </si>
+  <si>
+    <t>added extra for pin 13 LED</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1081,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1167,8 +1230,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="40">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1390,6 +1459,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -1590,7 +1683,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1634,6 +1727,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="43" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="38" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2064,36 +2175,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V92"/>
+  <dimension ref="A1:AA92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="18" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="12" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="5" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" customWidth="1"/>
+    <col min="17" max="17" width="2.85546875" customWidth="1"/>
     <col min="18" max="18" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.5703125" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" style="14" customWidth="1"/>
+    <col min="21" max="21" width="34.5703125" customWidth="1"/>
+    <col min="22" max="22" width="39.140625" customWidth="1"/>
+    <col min="23" max="23" width="38.5703125" customWidth="1"/>
+    <col min="27" max="27" width="3.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2106,57 +2222,57 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="P1" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>195</v>
-      </c>
       <c r="R1" s="7" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="T1" s="13" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="U1" s="7"/>
       <c r="V1" s="7" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2169,37 +2285,37 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="H3" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I3">
         <v>16.89</v>
       </c>
       <c r="O3" t="s">
-        <v>307</v>
-      </c>
-      <c r="Q3">
-        <v>80</v>
+        <v>297</v>
       </c>
       <c r="R3">
-        <f>B3*Q3</f>
+        <f>B3*AA3</f>
         <v>160</v>
       </c>
       <c r="T3" s="14">
         <f>R3*I3</f>
         <v>2702.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2212,14 +2328,11 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="H5" s="11">
         <v>44701</v>
@@ -2228,21 +2341,24 @@
         <v>16.46</v>
       </c>
       <c r="O5" t="s">
-        <v>308</v>
-      </c>
-      <c r="Q5">
-        <v>80</v>
+        <v>298</v>
       </c>
       <c r="R5">
-        <f>B5*Q5</f>
+        <f>B5*AA5</f>
         <v>80</v>
       </c>
       <c r="T5" s="14">
         <f>R5*I5</f>
         <v>1316.8000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2255,104 +2371,100 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
       <c r="F7" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="H7" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I7">
         <v>7</v>
       </c>
-      <c r="Q7">
-        <v>80</v>
-      </c>
       <c r="R7">
-        <f>B7*Q7</f>
+        <f>B7*AA7</f>
         <v>80</v>
       </c>
       <c r="T7" s="14">
         <f>R7*I7</f>
         <v>560</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="30">
         <v>8</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>316</v>
-      </c>
-      <c r="E9" t="s">
-        <v>18</v>
+        <v>306</v>
       </c>
       <c r="F9" t="s">
         <v>19</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="H9" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I9">
-        <v>0.36</v>
+        <v>0.15</v>
       </c>
       <c r="N9">
         <v>2069174</v>
       </c>
-      <c r="Q9">
-        <v>80</v>
-      </c>
       <c r="R9">
-        <f>B9*Q9</f>
+        <f>B9*AA9</f>
         <v>640</v>
       </c>
       <c r="S9">
-        <f>R9*1.05</f>
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="T9" s="14">
-        <f>S9*I9</f>
-        <v>241.92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+        <f t="shared" ref="T9:T16" si="0">S9*I9</f>
+        <v>100.5</v>
+      </c>
+      <c r="W9" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>181</v>
-      </c>
-      <c r="B10" s="18">
+        <v>173</v>
+      </c>
+      <c r="B10" s="30">
         <v>2</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>315</v>
-      </c>
-      <c r="E10" t="s">
-        <v>21</v>
+        <v>305</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="H10" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I10">
         <v>0.05</v>
@@ -2360,93 +2472,103 @@
       <c r="N10" s="26">
         <v>2280669</v>
       </c>
-      <c r="Q10">
-        <v>80</v>
-      </c>
       <c r="R10">
-        <f>B10*Q10</f>
+        <f>B10*AA10</f>
         <v>160</v>
       </c>
       <c r="S10">
-        <f t="shared" ref="S10:S70" si="0">R10*1.05</f>
+        <v>170</v>
+      </c>
+      <c r="T10" s="14">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+      <c r="W10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="B11" s="24">
+        <v>2</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>307</v>
+      </c>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="I11" s="23">
+        <v>0.09</v>
+      </c>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23" t="s">
+        <v>349</v>
+      </c>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23">
+        <v>2332787</v>
+      </c>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="R11" s="23">
+        <f>B11*AA11</f>
+        <v>160</v>
+      </c>
+      <c r="S11" s="23">
+        <f t="shared" ref="S11:S70" si="1">R11*1.05</f>
         <v>168</v>
       </c>
-      <c r="T10" s="14">
-        <f>S10*I10</f>
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>182</v>
-      </c>
-      <c r="B11" s="18">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>317</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="T11" s="32">
+        <f t="shared" si="0"/>
+        <v>15.12</v>
+      </c>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="H11" t="s">
-        <v>169</v>
-      </c>
-      <c r="I11">
-        <v>0.09</v>
-      </c>
-      <c r="N11">
-        <v>2332787</v>
-      </c>
-      <c r="Q11">
-        <v>80</v>
-      </c>
-      <c r="R11">
-        <f>B11*Q11</f>
-        <v>160</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="0"/>
-        <v>168</v>
-      </c>
-      <c r="T11" s="14">
-        <f>S11*I11</f>
-        <v>15.12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AA11" s="23">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="30">
         <v>2</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>318</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
+        <v>308</v>
       </c>
       <c r="F12" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="H12" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I12">
         <v>0.03</v>
@@ -2454,46 +2576,46 @@
       <c r="N12" s="26">
         <v>1414696</v>
       </c>
-      <c r="Q12">
-        <v>80</v>
-      </c>
       <c r="R12">
-        <f>B12*Q12</f>
+        <f>B12*AA12</f>
         <v>160</v>
       </c>
       <c r="S12">
+        <f t="shared" si="1"/>
+        <v>168</v>
+      </c>
+      <c r="T12" s="14">
         <f t="shared" si="0"/>
-        <v>168</v>
-      </c>
-      <c r="T12" s="14">
-        <f>S12*I12</f>
         <v>5.04</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W12" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="30">
         <v>4</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>319</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
+        <v>309</v>
       </c>
       <c r="F13" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="H13" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I13">
         <v>0.04</v>
@@ -2501,55 +2623,55 @@
       <c r="N13">
         <v>1759189</v>
       </c>
-      <c r="Q13">
-        <v>80</v>
-      </c>
       <c r="R13">
-        <f>B13*Q13</f>
+        <f>B13*AA13</f>
         <v>320</v>
       </c>
       <c r="S13">
+        <f t="shared" si="1"/>
+        <v>336</v>
+      </c>
+      <c r="T13" s="14">
         <f t="shared" si="0"/>
-        <v>336</v>
-      </c>
-      <c r="T13" s="14">
-        <f>S13*I13</f>
         <v>13.44</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W13" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="30">
         <v>2</v>
       </c>
       <c r="C14" t="s">
         <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>320</v>
-      </c>
-      <c r="E14" t="s">
-        <v>21</v>
+        <v>310</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="H14" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="I14">
         <v>0.18</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="K14" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="L14">
         <v>0.28000000000000003</v>
@@ -2558,98 +2680,98 @@
         <v>1432430</v>
       </c>
       <c r="O14" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="P14" t="s">
-        <v>322</v>
-      </c>
-      <c r="Q14">
-        <v>80</v>
+        <v>312</v>
       </c>
       <c r="R14">
-        <f>B14*Q14</f>
+        <f>B14*AA14</f>
         <v>160</v>
       </c>
       <c r="S14">
+        <f t="shared" si="1"/>
+        <v>168</v>
+      </c>
+      <c r="T14" s="14">
         <f t="shared" si="0"/>
-        <v>168</v>
-      </c>
-      <c r="T14" s="14">
-        <f>S14*I14</f>
         <v>30.24</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W14" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="18">
-        <v>26</v>
+      <c r="B15" s="30">
+        <v>28</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>317</v>
-      </c>
-      <c r="E15" t="s">
-        <v>21</v>
+        <v>307</v>
       </c>
       <c r="F15" t="s">
         <v>22</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>229</v>
+        <v>175</v>
       </c>
       <c r="H15" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I15">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="N15">
-        <v>1301717</v>
-      </c>
-      <c r="Q15">
-        <v>80</v>
+        <v>2280669</v>
       </c>
       <c r="R15">
-        <f>B15*Q15</f>
-        <v>2080</v>
+        <f>B15*AA15</f>
+        <v>2240</v>
       </c>
       <c r="S15">
+        <f t="shared" si="1"/>
+        <v>2352</v>
+      </c>
+      <c r="T15" s="14">
         <f t="shared" si="0"/>
-        <v>2184</v>
-      </c>
-      <c r="T15" s="14">
-        <f>S15*I15</f>
-        <v>87.36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+        <v>47.04</v>
+      </c>
+      <c r="W15" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>210</v>
-      </c>
-      <c r="B16" s="18">
+        <v>201</v>
+      </c>
+      <c r="B16" s="30">
         <v>3</v>
       </c>
       <c r="C16" t="s">
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>323</v>
-      </c>
-      <c r="E16" t="s">
-        <v>32</v>
+        <v>313</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="H16" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I16">
         <v>0.18</v>
@@ -2657,43 +2779,43 @@
       <c r="N16">
         <v>2068675</v>
       </c>
-      <c r="Q16">
-        <v>80</v>
-      </c>
       <c r="R16">
-        <f>B16*Q16</f>
+        <f>B16*AA16</f>
         <v>240</v>
       </c>
       <c r="S16">
+        <f t="shared" si="1"/>
+        <v>252</v>
+      </c>
+      <c r="T16" s="14">
         <f t="shared" si="0"/>
-        <v>252</v>
-      </c>
-      <c r="T16" s="14">
-        <f>S16*I16</f>
         <v>45.36</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W16" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="34">
         <v>1</v>
       </c>
       <c r="C18" t="s">
         <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>324</v>
-      </c>
-      <c r="E18" t="s">
-        <v>35</v>
+        <v>314</v>
       </c>
       <c r="F18" t="s">
         <v>36</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="H18" s="11">
         <v>44683</v>
@@ -2704,43 +2826,43 @@
       <c r="N18">
         <v>2319152</v>
       </c>
-      <c r="Q18">
-        <v>80</v>
-      </c>
       <c r="R18">
-        <f>B18*Q18</f>
+        <f>B18*AA18</f>
         <v>80</v>
       </c>
       <c r="S18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="T18" s="14">
         <f>S18*I18</f>
         <v>11.760000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W18" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA18">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B19" s="28">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D19" t="s">
-        <v>197</v>
-      </c>
-      <c r="E19" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="F19" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G19" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="H19" s="11">
         <v>44833</v>
@@ -2748,133 +2870,140 @@
       <c r="I19">
         <v>0.25</v>
       </c>
-      <c r="Q19">
-        <v>80</v>
-      </c>
       <c r="R19">
-        <f>B19*Q19</f>
+        <f>B19*AA19</f>
         <v>160</v>
       </c>
       <c r="S19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="T19" s="14">
         <f>S19*I19</f>
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W19" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="30">
         <v>2</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>325</v>
-      </c>
-      <c r="E20" t="s">
-        <v>39</v>
+        <v>315</v>
       </c>
       <c r="F20" t="s">
         <v>40</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="H20" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I20">
         <v>0.31</v>
       </c>
       <c r="N20" t="s">
-        <v>326</v>
-      </c>
-      <c r="Q20">
-        <v>80</v>
+        <v>316</v>
       </c>
       <c r="R20">
-        <f>B20*Q20</f>
+        <f>B20*AA20</f>
         <v>160</v>
       </c>
       <c r="S20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="T20" s="14">
         <f>S20*I20</f>
         <v>52.08</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W20" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA20">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>256</v>
-      </c>
-      <c r="B21" s="18">
-        <v>1</v>
+        <v>246</v>
+      </c>
+      <c r="B21" s="30">
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="D21" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="F21" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="H21" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I21">
         <v>0.1</v>
       </c>
+      <c r="K21" t="s">
+        <v>350</v>
+      </c>
       <c r="N21">
         <v>3796324</v>
       </c>
-      <c r="Q21">
-        <v>80</v>
-      </c>
       <c r="R21">
-        <f>B21*Q21</f>
-        <v>80</v>
+        <f>B21*AA21</f>
+        <v>240</v>
       </c>
       <c r="S21">
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>252</v>
       </c>
       <c r="T21" s="14">
         <f>S21*I21</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+        <v>25.200000000000003</v>
+      </c>
+      <c r="AA21">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>257</v>
-      </c>
-      <c r="B22" s="18">
+        <v>247</v>
+      </c>
+      <c r="B22" s="30">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="D22" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="F22" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="H22" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I22">
         <v>0.14000000000000001</v>
@@ -2882,11 +3011,8 @@
       <c r="N22">
         <v>2290332</v>
       </c>
-      <c r="Q22">
-        <v>80</v>
-      </c>
       <c r="R22">
-        <f>B22*Q22</f>
+        <f>B22*AA22</f>
         <v>80</v>
       </c>
       <c r="S22">
@@ -2896,31 +3022,31 @@
         <f>S22*I22</f>
         <v>14.000000000000002</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="AA22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="18">
-        <v>1</v>
+      <c r="B24" s="30">
+        <v>2</v>
       </c>
       <c r="C24" t="s">
         <v>42</v>
       </c>
       <c r="D24" t="s">
-        <v>329</v>
-      </c>
-      <c r="E24" t="s">
-        <v>44</v>
+        <v>319</v>
       </c>
       <c r="F24" t="s">
         <v>43</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="H24" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I24">
         <v>1.33</v>
@@ -2929,599 +3055,628 @@
         <v>1597013</v>
       </c>
       <c r="P24" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q24">
-        <v>80</v>
+        <v>226</v>
       </c>
       <c r="R24">
-        <f>B24*Q24</f>
-        <v>80</v>
+        <f>B24*AA24</f>
+        <v>160</v>
       </c>
       <c r="S24">
-        <f t="shared" si="0"/>
-        <v>84</v>
+        <f t="shared" si="1"/>
+        <v>168</v>
       </c>
       <c r="T24" s="14">
         <f>S24*I24</f>
-        <v>111.72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+        <v>223.44</v>
+      </c>
+      <c r="W24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA24">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="33">
         <v>1</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="D25" t="s">
-        <v>329</v>
-      </c>
-      <c r="E25" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="D25" s="35" t="s">
+        <v>319</v>
+      </c>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="G25" t="s">
-        <v>235</v>
-      </c>
-      <c r="H25" t="s">
-        <v>169</v>
-      </c>
-      <c r="I25">
+      <c r="G25" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="H25" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="I25" s="35">
         <v>1.33</v>
       </c>
-      <c r="N25">
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="M25" s="35"/>
+      <c r="N25" s="35">
         <v>1597013</v>
       </c>
-      <c r="P25" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q25">
-        <v>80</v>
+      <c r="O25" s="35"/>
+      <c r="P25" s="35" t="s">
+        <v>226</v>
       </c>
       <c r="R25">
-        <f>B25*Q25</f>
+        <f>B25*AA25</f>
         <v>80</v>
       </c>
       <c r="S25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="T25" s="14">
         <f>S25*I25</f>
         <v>111.72</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="Q26">
-        <v>80</v>
-      </c>
+      <c r="W25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="R26">
-        <f>B26*Q26</f>
+        <f>B26*AA26</f>
         <v>0</v>
       </c>
       <c r="S26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T26" s="14">
         <f>S26*I26</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="AA26">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B27" s="27">
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D27" t="s">
-        <v>202</v>
-      </c>
-      <c r="E27" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F27" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="H27" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I27">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="O27" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q27">
-        <v>80</v>
+        <v>299</v>
       </c>
       <c r="R27">
-        <f>B27*Q27</f>
+        <f>B27*AA27</f>
         <v>160</v>
       </c>
       <c r="S27" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="T27" s="14">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W27" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA27">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q29">
-        <v>80</v>
+        <v>178</v>
       </c>
       <c r="R29">
-        <f>B29*Q29</f>
+        <f>B29*AA29</f>
         <v>0</v>
       </c>
       <c r="S29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T29" s="14">
-        <f>S29*I29</f>
+        <f t="shared" ref="T29:T40" si="2">S29*I29</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="AA29">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>267</v>
-      </c>
-      <c r="B30" s="18">
+        <v>257</v>
+      </c>
+      <c r="B30" s="30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="D30" t="s">
-        <v>47</v>
-      </c>
-      <c r="E30" t="s">
-        <v>48</v>
+        <v>320</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="H30" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I30">
         <v>0.51</v>
       </c>
-      <c r="Q30">
-        <v>80</v>
+      <c r="N30">
+        <v>9731679</v>
       </c>
       <c r="R30">
-        <f>B30*Q30</f>
+        <f>B30*AA30</f>
         <v>240</v>
       </c>
       <c r="S30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>252</v>
       </c>
       <c r="T30" s="14">
-        <f>S30*I30</f>
+        <f t="shared" si="2"/>
         <v>128.52000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W30" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA30">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B31" s="18">
         <v>4</v>
       </c>
       <c r="C31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" t="s">
         <v>67</v>
       </c>
-      <c r="D31" t="s">
+      <c r="F31" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="G31" t="s">
+        <v>176</v>
+      </c>
+      <c r="R31">
+        <f>B31*AA31</f>
+        <v>320</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="1"/>
+        <v>336</v>
+      </c>
+      <c r="T31" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W31" t="s">
         <v>68</v>
       </c>
-      <c r="E31" t="s">
-        <v>69</v>
-      </c>
-      <c r="F31" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="G31" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q31">
-        <v>80</v>
-      </c>
-      <c r="R31">
-        <f>B31*Q31</f>
-        <v>320</v>
-      </c>
-      <c r="S31">
-        <f t="shared" si="0"/>
-        <v>336</v>
-      </c>
-      <c r="T31" s="14">
-        <f>S31*I31</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="AA31">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="B32" s="18">
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D32" t="s">
-        <v>75</v>
-      </c>
-      <c r="E32" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="G32" t="s">
+        <v>176</v>
+      </c>
+      <c r="R32">
+        <f>B32*AA32</f>
+        <v>160</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="1"/>
+        <v>168</v>
+      </c>
+      <c r="T32" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W32" t="s">
         <v>50</v>
       </c>
-      <c r="F32" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="G32" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q32">
-        <v>80</v>
-      </c>
-      <c r="R32">
-        <f>B32*Q32</f>
-        <v>160</v>
-      </c>
-      <c r="S32">
-        <f t="shared" si="0"/>
-        <v>168</v>
-      </c>
-      <c r="T32" s="14">
-        <f>S32*I32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="AA32">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B33" s="18">
         <v>1</v>
       </c>
       <c r="C33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" t="s">
         <v>71</v>
       </c>
-      <c r="D33" t="s">
+      <c r="F33" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="G33" t="s">
+        <v>176</v>
+      </c>
+      <c r="R33">
+        <f>B33*AA33</f>
+        <v>80</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="T33" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W33" t="s">
         <v>72</v>
       </c>
-      <c r="E33" t="s">
-        <v>73</v>
-      </c>
-      <c r="F33" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="G33" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q33">
-        <v>80</v>
-      </c>
-      <c r="R33">
-        <f>B33*Q33</f>
-        <v>80</v>
-      </c>
-      <c r="S33">
-        <f t="shared" si="0"/>
+      <c r="AA33">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>84</v>
-      </c>
-      <c r="T33" s="14">
-        <f>S33*I33</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>87</v>
       </c>
       <c r="B34" s="18">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D34" t="s">
-        <v>75</v>
-      </c>
-      <c r="E34" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="G34" t="s">
+        <v>176</v>
+      </c>
+      <c r="R34">
+        <f>B34*AA34</f>
+        <v>80</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="T34" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W34" t="s">
         <v>50</v>
       </c>
-      <c r="F34" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="G34" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q34">
-        <v>80</v>
-      </c>
-      <c r="R34">
-        <f>B34*Q34</f>
-        <v>80</v>
-      </c>
-      <c r="S34">
-        <f t="shared" si="0"/>
-        <v>84</v>
-      </c>
-      <c r="T34" s="14">
-        <f>S34*I34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="AA34">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" s="18">
+        <v>90</v>
+      </c>
+      <c r="B35" s="30">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D35" t="s">
-        <v>75</v>
-      </c>
-      <c r="E35" t="s">
-        <v>50</v>
+        <v>321</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="H35" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I35">
         <v>0.11</v>
       </c>
-      <c r="Q35">
-        <v>80</v>
+      <c r="N35">
+        <v>1022248</v>
       </c>
       <c r="R35">
-        <f>B35*Q35</f>
+        <f>B35*AA35</f>
         <v>80</v>
       </c>
       <c r="S35">
         <v>100</v>
       </c>
       <c r="T35" s="14">
-        <f>S35*I35</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W35" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B36" s="18">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="G36" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q36">
-        <v>80</v>
+        <v>176</v>
       </c>
       <c r="R36">
-        <f>B36*Q36</f>
+        <f>B36*AA36</f>
         <v>80</v>
       </c>
       <c r="S36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="T36" s="14">
-        <f>S36*I36</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W36" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA36">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B37" s="18">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D37" t="s">
-        <v>213</v>
-      </c>
-      <c r="E37" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="G37" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q37">
-        <v>80</v>
+        <v>176</v>
       </c>
       <c r="R37">
-        <f>B37*Q37</f>
+        <f>B37*AA37</f>
         <v>80</v>
       </c>
       <c r="S37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="T37" s="14">
-        <f>S37*I37</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W37" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA37">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B38" s="18">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D38" t="s">
         <v>47</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="G38" t="s">
+        <v>176</v>
+      </c>
+      <c r="R38">
+        <f>B38*AA38</f>
+        <v>80</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="T38" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W38" t="s">
         <v>48</v>
       </c>
-      <c r="F38" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="G38" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q38">
-        <v>80</v>
-      </c>
-      <c r="R38">
-        <f>B38*Q38</f>
-        <v>80</v>
-      </c>
-      <c r="S38">
-        <f t="shared" si="0"/>
-        <v>84</v>
-      </c>
-      <c r="T38" s="14">
-        <f>S38*I38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="AA38">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>270</v>
-      </c>
-      <c r="B39" s="18">
+        <v>260</v>
+      </c>
+      <c r="B39" s="30">
         <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>273</v>
-      </c>
-      <c r="E39" t="s">
-        <v>48</v>
+        <v>263</v>
+      </c>
+      <c r="D39" t="s">
+        <v>322</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="H39" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I39">
         <v>0.48</v>
       </c>
-      <c r="Q39">
-        <v>80</v>
+      <c r="N39">
+        <v>1022262</v>
       </c>
       <c r="R39">
-        <f>B39*Q39</f>
+        <f>B39*AA39</f>
         <v>480</v>
       </c>
       <c r="S39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>504</v>
       </c>
       <c r="T39" s="14">
-        <f>S39*I39</f>
+        <f t="shared" si="2"/>
         <v>241.92</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W39" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA39">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>271</v>
-      </c>
-      <c r="B40" s="18">
+        <v>261</v>
+      </c>
+      <c r="B40" s="30">
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>274</v>
-      </c>
-      <c r="E40" t="s">
-        <v>69</v>
+        <v>264</v>
+      </c>
+      <c r="D40" t="s">
+        <v>323</v>
       </c>
       <c r="F40" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="G40" t="s">
-        <v>275</v>
+        <v>176</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>265</v>
       </c>
       <c r="H40" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I40">
         <v>0.28999999999999998</v>
       </c>
-      <c r="Q40">
-        <v>80</v>
+      <c r="N40">
+        <v>1593469</v>
       </c>
       <c r="R40">
-        <f>B40*Q40</f>
+        <f>B40*AA40</f>
         <v>480</v>
       </c>
       <c r="S40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>504</v>
       </c>
       <c r="T40" s="14">
-        <f>S40*I40</f>
+        <f t="shared" si="2"/>
         <v>146.16</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W40" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA40">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="18">
+      <c r="B43" s="27">
         <v>1</v>
       </c>
       <c r="C43" t="s">
@@ -3530,32 +3685,26 @@
       <c r="D43" t="s">
         <v>53</v>
       </c>
-      <c r="E43" t="s">
-        <v>54</v>
-      </c>
       <c r="F43" t="s">
         <v>55</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="H43" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I43">
         <v>0.96199999999999997</v>
       </c>
       <c r="J43" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="O43" t="s">
-        <v>310</v>
-      </c>
-      <c r="Q43">
-        <v>80</v>
+        <v>300</v>
       </c>
       <c r="R43">
-        <f>B43*Q43</f>
+        <f>B43*AA43</f>
         <v>80</v>
       </c>
       <c r="S43">
@@ -3565,44 +3714,47 @@
         <f>S43*I43</f>
         <v>86.58</v>
       </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W43" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA43">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="18">
-        <v>2</v>
+      <c r="B44" s="30">
+        <v>1</v>
       </c>
       <c r="C44" t="s">
         <v>59</v>
       </c>
       <c r="D44" t="s">
-        <v>60</v>
-      </c>
-      <c r="E44" t="s">
+        <v>324</v>
+      </c>
+      <c r="F44" t="s">
         <v>61</v>
       </c>
-      <c r="F44" t="s">
-        <v>62</v>
-      </c>
-      <c r="G44" t="s">
-        <v>245</v>
+      <c r="G44" s="10" t="s">
+        <v>235</v>
       </c>
       <c r="H44" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I44">
         <v>0.44</v>
       </c>
       <c r="J44" t="s">
-        <v>246</v>
-      </c>
-      <c r="Q44">
-        <v>80</v>
+        <v>236</v>
+      </c>
+      <c r="N44">
+        <v>2784974</v>
       </c>
       <c r="R44">
-        <f>B44*Q44</f>
-        <v>160</v>
+        <f>B44*AA44</f>
+        <v>80</v>
       </c>
       <c r="S44">
         <v>100</v>
@@ -3611,412 +3763,430 @@
         <f>S44*I44</f>
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W44" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA44">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="30">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="18">
-        <v>2</v>
-      </c>
-      <c r="C45" t="s">
-        <v>64</v>
-      </c>
       <c r="D45" t="s">
-        <v>64</v>
-      </c>
-      <c r="E45" t="s">
+        <v>325</v>
+      </c>
+      <c r="F45" t="s">
         <v>65</v>
       </c>
-      <c r="F45" t="s">
-        <v>66</v>
-      </c>
-      <c r="G45" t="s">
-        <v>247</v>
+      <c r="G45" s="10" t="s">
+        <v>237</v>
       </c>
       <c r="H45" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I45">
         <v>0.46</v>
       </c>
-      <c r="Q45">
-        <v>80</v>
+      <c r="N45">
+        <v>2293774</v>
       </c>
       <c r="R45">
-        <f>B45*Q45</f>
+        <f>B45*AA45</f>
         <v>160</v>
       </c>
       <c r="S45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="T45" s="14">
         <f>S45*I45</f>
         <v>77.28</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W45" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>248</v>
-      </c>
-      <c r="B46" s="18">
+        <v>238</v>
+      </c>
+      <c r="B46" s="30">
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="D46" t="s">
+        <v>326</v>
+      </c>
+      <c r="F46" t="s">
         <v>76</v>
       </c>
-      <c r="E46" t="s">
-        <v>77</v>
-      </c>
-      <c r="F46" t="s">
-        <v>78</v>
-      </c>
       <c r="G46" s="10" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="H46" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I46">
         <v>0.26</v>
       </c>
-      <c r="Q46">
-        <v>80</v>
+      <c r="N46">
+        <v>2008019</v>
       </c>
       <c r="R46">
-        <f>B46*Q46</f>
+        <f>B46*AA46</f>
         <v>320</v>
       </c>
       <c r="S46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>336</v>
       </c>
       <c r="T46" s="14">
         <f>S46*I46</f>
         <v>87.36</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W46" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA46">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>185</v>
-      </c>
-      <c r="B47" s="18">
+        <v>177</v>
+      </c>
+      <c r="B47" s="30">
         <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D47" t="s">
-        <v>79</v>
-      </c>
-      <c r="E47" t="s">
-        <v>80</v>
+        <v>327</v>
       </c>
       <c r="F47" t="s">
-        <v>81</v>
-      </c>
-      <c r="G47" t="s">
-        <v>251</v>
+        <v>78</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>241</v>
       </c>
       <c r="H47" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I47">
         <v>0.45</v>
       </c>
-      <c r="Q47">
-        <v>80</v>
+      <c r="N47">
+        <v>2008020</v>
       </c>
       <c r="R47">
-        <f>B47*Q47</f>
+        <f>B47*AA47</f>
         <v>160</v>
       </c>
       <c r="S47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="T47" s="14">
         <f>S47*I47</f>
         <v>75.600000000000009</v>
       </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W47" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA47">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>253</v>
-      </c>
-      <c r="B51" s="18">
+        <v>243</v>
+      </c>
+      <c r="B51" s="30">
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="D51" t="s">
-        <v>56</v>
-      </c>
-      <c r="E51" t="s">
-        <v>57</v>
+        <v>328</v>
       </c>
       <c r="F51" t="s">
         <v>55</v>
       </c>
-      <c r="G51" t="s">
-        <v>252</v>
+      <c r="G51" s="10" t="s">
+        <v>242</v>
       </c>
       <c r="H51" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I51">
         <v>0.16</v>
       </c>
-      <c r="Q51">
-        <v>80</v>
+      <c r="N51">
+        <v>1462926</v>
       </c>
       <c r="R51">
-        <f>B51*Q51</f>
+        <f>B51*AA51</f>
         <v>240</v>
       </c>
       <c r="S51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>252</v>
       </c>
       <c r="T51" s="14">
-        <f>S51*I51</f>
+        <f t="shared" ref="T51:T56" si="3">S51*I51</f>
         <v>40.32</v>
       </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W51" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA51">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>265</v>
-      </c>
-      <c r="B52" s="18">
+        <v>255</v>
+      </c>
+      <c r="B52" s="30">
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="D52" t="s">
-        <v>75</v>
-      </c>
-      <c r="E52" t="s">
-        <v>50</v>
+        <v>329</v>
       </c>
       <c r="F52" t="s">
         <v>51</v>
       </c>
-      <c r="G52" t="s">
-        <v>264</v>
+      <c r="G52" s="10" t="s">
+        <v>254</v>
       </c>
       <c r="H52" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I52">
         <v>0.17</v>
       </c>
-      <c r="Q52">
-        <v>80</v>
+      <c r="N52">
+        <v>1462950</v>
       </c>
       <c r="R52">
-        <f>B52*Q52</f>
+        <f>B52*AA52</f>
         <v>240</v>
       </c>
       <c r="S52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>252</v>
       </c>
       <c r="T52" s="14">
-        <f>S52*I52</f>
+        <f t="shared" si="3"/>
         <v>42.84</v>
       </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W52" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA52">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>82</v>
-      </c>
-      <c r="B53" s="18">
+        <v>79</v>
+      </c>
+      <c r="B53" s="29">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D53" t="s">
-        <v>72</v>
-      </c>
-      <c r="E53" t="s">
+        <v>71</v>
+      </c>
+      <c r="F53" t="s">
         <v>73</v>
       </c>
-      <c r="F53" t="s">
-        <v>74</v>
-      </c>
       <c r="G53" s="10" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="H53" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I53">
         <v>0.38800000000000001</v>
       </c>
       <c r="O53" t="s">
-        <v>312</v>
-      </c>
-      <c r="Q53">
-        <v>80</v>
+        <v>302</v>
       </c>
       <c r="R53">
-        <f>B53*Q53</f>
+        <f>B53*AA53</f>
         <v>80</v>
       </c>
       <c r="S53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="T53" s="14">
-        <f>S53*I53</f>
+        <f t="shared" si="3"/>
         <v>32.591999999999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W53" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA53">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B54" s="19">
         <v>2</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F54" s="15" t="s">
         <v>51</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q54" s="15">
-        <v>80</v>
+        <v>245</v>
       </c>
       <c r="R54" s="15">
-        <f>B54*Q54</f>
+        <f>B54*AA54</f>
         <v>160</v>
       </c>
       <c r="S54" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="T54" s="16">
-        <f>S54*I54</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W54" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA54" s="15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B55" s="19">
         <v>2</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="15" t="s">
-        <v>84</v>
-      </c>
       <c r="F55" s="15" t="s">
         <v>55</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q55" s="15">
-        <v>80</v>
+        <v>245</v>
       </c>
       <c r="R55" s="15">
-        <f>B55*Q55</f>
+        <f>B55*AA55</f>
         <v>160</v>
       </c>
       <c r="S55" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="T55" s="16">
-        <f>S55*I55</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:20" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W55" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA55" s="15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B56" s="19">
         <v>1</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E56" s="15" t="s">
-        <v>48</v>
-      </c>
       <c r="F56" s="15" t="s">
         <v>49</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q56" s="15">
-        <v>80</v>
+        <v>245</v>
       </c>
       <c r="R56" s="15">
-        <f>B56*Q56</f>
+        <f>B56*AA56</f>
         <v>80</v>
       </c>
       <c r="S56" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="T56" s="16">
-        <f>S56*I56</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W56" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA56" s="15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B58" s="20">
         <v>2</v>
       </c>
       <c r="C58" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F58" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D58" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="E58" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>99</v>
-      </c>
       <c r="G58" s="8" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
@@ -4027,383 +4197,407 @@
       <c r="N58" s="8"/>
       <c r="O58" s="8"/>
       <c r="P58" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+      <c r="W58" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" s="30">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>98</v>
+      </c>
+      <c r="D60" t="s">
+        <v>330</v>
+      </c>
+      <c r="F60" t="s">
         <v>100</v>
       </c>
-      <c r="B60" s="18">
-        <v>1</v>
-      </c>
-      <c r="C60" t="s">
-        <v>101</v>
-      </c>
-      <c r="D60" t="s">
-        <v>101</v>
-      </c>
-      <c r="E60" t="s">
-        <v>102</v>
-      </c>
-      <c r="F60" t="s">
-        <v>103</v>
-      </c>
-      <c r="G60" t="s">
-        <v>278</v>
+      <c r="G60" s="10" t="s">
+        <v>268</v>
       </c>
       <c r="H60" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I60">
         <v>1.37</v>
       </c>
-      <c r="Q60">
-        <v>80</v>
+      <c r="N60">
+        <v>8648255</v>
       </c>
       <c r="R60">
-        <f>B60*Q60</f>
+        <f>B60*AA60</f>
         <v>80</v>
       </c>
       <c r="S60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="T60" s="14">
         <f>S60*I60</f>
         <v>115.08000000000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W60" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA60">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>101</v>
+      </c>
+      <c r="B62" s="30">
+        <v>2</v>
+      </c>
+      <c r="C62" t="s">
+        <v>102</v>
+      </c>
+      <c r="D62" t="s">
+        <v>331</v>
+      </c>
+      <c r="F62" t="s">
         <v>104</v>
       </c>
-      <c r="B62" s="18">
-        <v>2</v>
-      </c>
-      <c r="C62" t="s">
-        <v>105</v>
-      </c>
-      <c r="D62" t="s">
-        <v>106</v>
-      </c>
-      <c r="E62" t="s">
-        <v>107</v>
-      </c>
-      <c r="F62" t="s">
-        <v>108</v>
-      </c>
-      <c r="G62" t="s">
-        <v>279</v>
+      <c r="G62" s="10" t="s">
+        <v>269</v>
       </c>
       <c r="H62" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I62">
         <v>0.04</v>
       </c>
-      <c r="Q62">
-        <v>80</v>
+      <c r="N62">
+        <v>1576464</v>
       </c>
       <c r="R62">
-        <f>B62*Q62</f>
+        <f>B62*AA62</f>
         <v>160</v>
       </c>
       <c r="S62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="T62" s="14">
         <f>S62*I62</f>
         <v>6.72</v>
       </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W62" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA62">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>262</v>
-      </c>
-      <c r="B63" s="18">
+        <v>252</v>
+      </c>
+      <c r="B63" s="30">
         <v>4</v>
       </c>
       <c r="C63" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D63" t="s">
-        <v>106</v>
-      </c>
-      <c r="E63" t="s">
-        <v>107</v>
+        <v>332</v>
       </c>
       <c r="F63" t="s">
-        <v>108</v>
-      </c>
-      <c r="G63" t="s">
-        <v>280</v>
+        <v>104</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>270</v>
       </c>
       <c r="H63" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I63">
         <v>0.04</v>
       </c>
-      <c r="Q63">
-        <v>80</v>
+      <c r="N63">
+        <v>1576452</v>
       </c>
       <c r="R63">
-        <f>B63*Q63</f>
+        <f>B63*AA63</f>
         <v>320</v>
       </c>
       <c r="S63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>336</v>
       </c>
       <c r="T63" s="14">
         <f>S63*I63</f>
         <v>13.44</v>
       </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W63" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA63">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>110</v>
-      </c>
-      <c r="B64" s="18">
+        <v>106</v>
+      </c>
+      <c r="B64" s="30">
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D64" t="s">
-        <v>106</v>
-      </c>
-      <c r="E64" t="s">
-        <v>107</v>
+        <v>333</v>
       </c>
       <c r="F64" t="s">
-        <v>108</v>
-      </c>
-      <c r="G64" t="s">
-        <v>281</v>
+        <v>104</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>271</v>
       </c>
       <c r="H64" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I64">
         <v>0.02</v>
       </c>
-      <c r="Q64">
-        <v>80</v>
+      <c r="N64">
+        <v>2861558</v>
       </c>
       <c r="R64">
-        <f>B64*Q64</f>
+        <f>B64*AA64</f>
         <v>240</v>
       </c>
       <c r="S64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>252</v>
       </c>
       <c r="T64" s="14">
         <f>S64*I64</f>
         <v>5.04</v>
       </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W64" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA64">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>263</v>
-      </c>
-      <c r="B65" s="18">
+        <v>253</v>
+      </c>
+      <c r="B65" s="30">
         <v>18</v>
       </c>
       <c r="C65" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D65" t="s">
-        <v>106</v>
-      </c>
-      <c r="E65" t="s">
-        <v>107</v>
+        <v>334</v>
       </c>
       <c r="F65" t="s">
-        <v>108</v>
-      </c>
-      <c r="G65" t="s">
-        <v>282</v>
+        <v>104</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>272</v>
       </c>
       <c r="H65" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I65">
         <v>0.01</v>
       </c>
-      <c r="Q65">
-        <v>80</v>
+      <c r="N65">
+        <v>2332071</v>
       </c>
       <c r="R65">
-        <f>B65*Q65</f>
+        <f>B65*AA65</f>
         <v>1440</v>
       </c>
       <c r="S65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1512</v>
       </c>
       <c r="T65" s="14">
         <f>S65*I65</f>
         <v>15.120000000000001</v>
       </c>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W65" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA65">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>113</v>
-      </c>
-      <c r="B66" s="18">
+        <v>109</v>
+      </c>
+      <c r="B66" s="30">
         <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D66" t="s">
-        <v>106</v>
-      </c>
-      <c r="E66" t="s">
-        <v>107</v>
+        <v>335</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="G66" t="s">
-        <v>283</v>
+        <v>208</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>273</v>
       </c>
       <c r="H66" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I66">
         <v>0.01</v>
       </c>
-      <c r="Q66">
-        <v>80</v>
+      <c r="N66">
+        <v>2670094</v>
       </c>
       <c r="R66">
-        <f>B66*Q66</f>
+        <f>B66*AA66</f>
         <v>160</v>
       </c>
       <c r="S66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="T66" s="14">
         <f>S66*I66</f>
         <v>1.68</v>
       </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W66" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA66">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>115</v>
-      </c>
-      <c r="B67" s="18">
+        <v>111</v>
+      </c>
+      <c r="B67" s="30">
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D67" t="s">
-        <v>106</v>
-      </c>
-      <c r="E67" t="s">
-        <v>107</v>
+        <v>336</v>
       </c>
       <c r="F67" t="s">
-        <v>108</v>
-      </c>
-      <c r="G67" t="s">
-        <v>284</v>
+        <v>104</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>274</v>
       </c>
       <c r="H67" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I67">
         <v>0.01</v>
       </c>
-      <c r="Q67">
-        <v>80</v>
+      <c r="N67" t="s">
+        <v>337</v>
       </c>
       <c r="R67">
-        <f>B67*Q67</f>
+        <f>B67*AA67</f>
         <v>320</v>
       </c>
       <c r="S67" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="T67" s="14">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W67" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA67">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>117</v>
-      </c>
-      <c r="B68" s="18">
+        <v>113</v>
+      </c>
+      <c r="B68" s="30">
         <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D68" t="s">
-        <v>106</v>
-      </c>
-      <c r="E68" t="s">
-        <v>107</v>
+        <v>338</v>
       </c>
       <c r="F68" t="s">
-        <v>108</v>
-      </c>
-      <c r="G68" t="s">
-        <v>286</v>
+        <v>104</v>
+      </c>
+      <c r="G68" s="10" t="s">
+        <v>276</v>
       </c>
       <c r="H68" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I68">
         <v>0.01</v>
       </c>
-      <c r="Q68">
-        <v>80</v>
+      <c r="N68">
+        <v>2447627</v>
       </c>
       <c r="R68">
-        <f>B68*Q68</f>
+        <f>B68*AA68</f>
         <v>240</v>
       </c>
       <c r="S68">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>252</v>
       </c>
       <c r="T68" s="14">
         <f>S68*I68</f>
         <v>2.52</v>
       </c>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W68" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA68">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>119</v>
-      </c>
-      <c r="B70" s="18">
+        <v>115</v>
+      </c>
+      <c r="B70" s="36">
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D70" t="s">
-        <v>121</v>
-      </c>
-      <c r="E70" t="s">
-        <v>122</v>
+        <v>339</v>
       </c>
       <c r="F70" t="s">
-        <v>123</v>
-      </c>
-      <c r="G70" t="s">
-        <v>287</v>
+        <v>118</v>
+      </c>
+      <c r="G70" s="10" t="s">
+        <v>277</v>
       </c>
       <c r="H70" s="11">
         <v>44823</v>
@@ -4411,52 +4605,58 @@
       <c r="I70">
         <v>0.85</v>
       </c>
-      <c r="Q70">
-        <v>80</v>
+      <c r="N70">
+        <v>3778050</v>
       </c>
       <c r="R70">
-        <f>B70*Q70</f>
+        <f>B70*AA70</f>
         <v>80</v>
       </c>
       <c r="S70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="T70" s="14">
         <f>S70*I70</f>
         <v>71.399999999999991</v>
       </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W70" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA70">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>209</v>
-      </c>
-      <c r="B71" s="18">
+        <v>200</v>
+      </c>
+      <c r="B71" s="30">
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D71" t="s">
-        <v>206</v>
+        <v>340</v>
       </c>
       <c r="F71" t="s">
-        <v>207</v>
-      </c>
-      <c r="G71" t="s">
-        <v>288</v>
+        <v>198</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>278</v>
       </c>
       <c r="H71" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I71">
         <v>0.21</v>
       </c>
-      <c r="Q71">
-        <v>80</v>
+      <c r="N71" t="s">
+        <v>341</v>
       </c>
       <c r="R71">
-        <f>B71*Q71</f>
+        <f>B71*AA71</f>
         <v>160</v>
       </c>
       <c r="S71">
@@ -4466,81 +4666,81 @@
         <f>S71*I71</f>
         <v>42</v>
       </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="AA71">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B74" s="18">
         <v>2</v>
       </c>
       <c r="C74" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D74" t="s">
-        <v>125</v>
-      </c>
-      <c r="E74" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F74" t="s">
-        <v>127</v>
-      </c>
-      <c r="G74" t="s">
-        <v>289</v>
+        <v>122</v>
+      </c>
+      <c r="G74" s="10" t="s">
+        <v>279</v>
       </c>
       <c r="H74" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="I74">
         <v>4</v>
       </c>
-      <c r="J74" t="s">
-        <v>291</v>
+      <c r="J74" s="10" t="s">
+        <v>281</v>
       </c>
       <c r="K74" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="L74">
         <v>1.66</v>
       </c>
-      <c r="Q74">
-        <v>80</v>
-      </c>
       <c r="R74">
-        <f>B74*Q74</f>
+        <f>B74*AA74</f>
         <v>160</v>
       </c>
       <c r="S74">
-        <f t="shared" ref="S74:S86" si="1">R74*1.05</f>
+        <f t="shared" ref="S74:S86" si="4">R74*1.05</f>
         <v>168</v>
       </c>
       <c r="T74" s="14">
         <f>S74*I74</f>
         <v>672</v>
       </c>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W74" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA74">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>128</v>
-      </c>
-      <c r="B76" s="18">
+        <v>123</v>
+      </c>
+      <c r="B76" s="30">
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D76" t="s">
-        <v>129</v>
-      </c>
-      <c r="E76" t="s">
-        <v>126</v>
+        <v>342</v>
       </c>
       <c r="F76" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="H76" s="11">
         <v>44732</v>
@@ -4548,20 +4748,20 @@
       <c r="I76">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="J76" t="s">
-        <v>303</v>
+      <c r="J76" s="10" t="s">
+        <v>293</v>
       </c>
       <c r="K76" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="L76">
         <v>0.4</v>
       </c>
-      <c r="Q76">
-        <v>80</v>
+      <c r="N76" t="s">
+        <v>343</v>
       </c>
       <c r="R76">
-        <f>B76*Q76</f>
+        <f>B76*AA76</f>
         <v>80</v>
       </c>
       <c r="S76">
@@ -4571,456 +4771,473 @@
         <f>S76*L76</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W76" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA76">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" s="23" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B77" s="24">
         <v>2</v>
       </c>
       <c r="C77" s="23" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D77" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="E77" s="23" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F77" s="23" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G77" s="23" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="H77" s="5">
         <v>45089</v>
       </c>
       <c r="I77" s="23" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="J77" s="23"/>
       <c r="K77" s="23"/>
       <c r="L77" s="23"/>
-      <c r="Q77">
-        <v>80</v>
-      </c>
       <c r="R77">
-        <f>B77*Q77</f>
+        <f>B77*AA77</f>
         <v>160</v>
       </c>
       <c r="S77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>168</v>
       </c>
-      <c r="T77" s="14" t="e">
-        <f>S77*#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W77" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA77">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>135</v>
-      </c>
-      <c r="B78" s="18">
+        <v>130</v>
+      </c>
+      <c r="B78" s="30">
         <v>2</v>
       </c>
       <c r="C78">
         <v>4094</v>
       </c>
-      <c r="D78">
-        <v>4094</v>
-      </c>
-      <c r="E78" t="s">
-        <v>136</v>
+      <c r="D78" t="s">
+        <v>344</v>
       </c>
       <c r="F78" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="H78" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I78">
         <v>0.47099999999999997</v>
       </c>
-      <c r="J78" t="s">
-        <v>172</v>
+      <c r="J78" s="10" t="s">
+        <v>164</v>
       </c>
       <c r="K78" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="L78">
         <v>0.55000000000000004</v>
       </c>
-      <c r="Q78">
-        <v>80</v>
+      <c r="N78">
+        <v>1201297</v>
       </c>
       <c r="R78">
-        <f>B78*Q78</f>
+        <f>B78*AA78</f>
         <v>160</v>
       </c>
       <c r="S78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>168</v>
       </c>
       <c r="T78" s="14">
         <f>S78*I78</f>
         <v>79.128</v>
       </c>
-    </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W78" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA78">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>138</v>
-      </c>
-      <c r="B79" s="18">
+        <v>133</v>
+      </c>
+      <c r="B79" s="30">
         <v>1</v>
       </c>
       <c r="C79">
         <v>4069</v>
       </c>
       <c r="D79" t="s">
-        <v>139</v>
-      </c>
-      <c r="E79" t="s">
-        <v>140</v>
+        <v>345</v>
       </c>
       <c r="F79" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="G79" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H79" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I79">
         <v>0.48699999999999999</v>
       </c>
-      <c r="J79" t="s">
-        <v>174</v>
+      <c r="J79" s="10" t="s">
+        <v>166</v>
       </c>
       <c r="K79" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="L79">
         <v>0.56999999999999995</v>
       </c>
-      <c r="Q79">
-        <v>80</v>
+      <c r="N79">
+        <v>1201295</v>
       </c>
       <c r="R79">
-        <f>B79*Q79</f>
+        <f>B79*AA79</f>
         <v>80</v>
       </c>
       <c r="S79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>84</v>
       </c>
       <c r="T79" s="14">
         <f>S79*I79</f>
         <v>40.908000000000001</v>
       </c>
-    </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W79" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA79">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>142</v>
-      </c>
-      <c r="B80" s="18">
+        <v>136</v>
+      </c>
+      <c r="B80" s="30">
         <v>4</v>
       </c>
       <c r="C80">
         <v>4081</v>
       </c>
       <c r="D80" t="s">
-        <v>143</v>
-      </c>
-      <c r="E80" t="s">
-        <v>140</v>
+        <v>346</v>
       </c>
       <c r="F80" t="s">
-        <v>144</v>
-      </c>
-      <c r="J80" t="s">
-        <v>175</v>
+        <v>137</v>
+      </c>
+      <c r="J80" s="10" t="s">
+        <v>167</v>
       </c>
       <c r="K80" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="L80">
         <v>0.56999999999999995</v>
       </c>
-      <c r="Q80">
-        <v>80</v>
+      <c r="N80">
+        <v>1085290</v>
       </c>
       <c r="R80">
-        <f>B80*Q80</f>
+        <f>B80*AA80</f>
         <v>320</v>
       </c>
       <c r="S80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>336</v>
       </c>
       <c r="T80" s="14">
         <f>S80*L80</f>
         <v>191.51999999999998</v>
       </c>
-    </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W80" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA80">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>145</v>
-      </c>
-      <c r="B81" s="18">
+        <v>138</v>
+      </c>
+      <c r="B81" s="30">
         <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D81" t="s">
-        <v>147</v>
-      </c>
-      <c r="E81" t="s">
+        <v>347</v>
+      </c>
+      <c r="F81" t="s">
         <v>140</v>
       </c>
-      <c r="F81" t="s">
-        <v>148</v>
-      </c>
-      <c r="J81" t="s">
-        <v>176</v>
+      <c r="J81" s="10" t="s">
+        <v>168</v>
       </c>
       <c r="K81" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="L81">
         <v>0.49</v>
       </c>
-      <c r="Q81">
-        <v>80</v>
+      <c r="N81">
+        <v>1085331</v>
       </c>
       <c r="R81">
-        <f>B81*Q81</f>
+        <f>B81*AA81</f>
         <v>160</v>
       </c>
       <c r="S81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>168</v>
       </c>
       <c r="T81" s="14">
         <f>S81*L81</f>
         <v>82.32</v>
       </c>
-    </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W81" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>149</v>
-      </c>
-      <c r="B82" s="18">
+        <v>141</v>
+      </c>
+      <c r="B82" s="28">
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D82" t="s">
-        <v>150</v>
-      </c>
-      <c r="E82" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="F82" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="H82" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q82">
-        <v>80</v>
+        <v>169</v>
       </c>
       <c r="R82">
-        <f>B82*Q82</f>
+        <f>B82*AA82</f>
         <v>80</v>
       </c>
       <c r="S82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>84</v>
       </c>
       <c r="T82" s="14">
         <f>S82*I82</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W82" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA82">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>153</v>
-      </c>
-      <c r="B83" s="18">
+        <v>145</v>
+      </c>
+      <c r="B83" s="27">
         <v>3</v>
       </c>
       <c r="C83" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D83" t="s">
-        <v>155</v>
-      </c>
-      <c r="E83" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="F83" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="H83" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I83">
         <v>0.28799999999999998</v>
       </c>
       <c r="O83" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q83">
-        <v>80</v>
+        <v>301</v>
       </c>
       <c r="R83">
-        <f>B83*Q83</f>
+        <f>B83*AA83</f>
         <v>240</v>
       </c>
       <c r="S83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>252</v>
       </c>
       <c r="T83" s="14">
         <f>S83*I83</f>
         <v>72.575999999999993</v>
       </c>
-    </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W83" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA83">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>157</v>
-      </c>
-      <c r="B84" s="18">
+        <v>149</v>
+      </c>
+      <c r="B84" s="30">
         <v>3</v>
       </c>
       <c r="C84" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="D84" t="s">
-        <v>297</v>
-      </c>
-      <c r="E84" t="s">
-        <v>140</v>
+        <v>348</v>
       </c>
       <c r="F84" t="s">
-        <v>298</v>
-      </c>
-      <c r="G84" t="s">
-        <v>295</v>
+        <v>288</v>
+      </c>
+      <c r="G84" s="10" t="s">
+        <v>285</v>
       </c>
       <c r="H84" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I84">
         <v>1.1000000000000001</v>
       </c>
       <c r="J84" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="K84" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q84">
-        <v>80</v>
+        <v>284</v>
+      </c>
+      <c r="N84">
+        <v>2774608</v>
       </c>
       <c r="R84">
-        <f>B84*Q84</f>
+        <f>B84*AA84</f>
         <v>240</v>
       </c>
       <c r="S84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>252</v>
       </c>
       <c r="T84" s="14">
         <f>S84*I84</f>
         <v>277.20000000000005</v>
       </c>
-    </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="Q85">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W84" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA84">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA85">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>158</v>
-      </c>
-      <c r="B86" s="18">
+        <v>150</v>
+      </c>
+      <c r="B86" s="30">
         <v>2</v>
       </c>
       <c r="C86" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D86" t="s">
-        <v>160</v>
-      </c>
-      <c r="E86" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="F86" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="G86" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="H86" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="I86">
         <v>1.27</v>
       </c>
-      <c r="J86" t="s">
-        <v>301</v>
+      <c r="J86" s="10" t="s">
+        <v>291</v>
       </c>
       <c r="K86" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="L86">
         <v>1.52</v>
       </c>
-      <c r="Q86">
-        <v>80</v>
-      </c>
       <c r="R86">
-        <f>B86*Q86</f>
+        <f>B86*AA86</f>
         <v>160</v>
       </c>
       <c r="S86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>168</v>
       </c>
       <c r="T86" s="14">
         <f>S86*L86</f>
         <v>255.36</v>
       </c>
-    </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W86" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA86">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="C89" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="R92" s="25" t="s">
-        <v>304</v>
-      </c>
-      <c r="T92" s="14" t="e">
+        <v>294</v>
+      </c>
+      <c r="T92" s="14">
         <f xml:space="preserve"> SUM(T3:T86)</f>
-        <v>#REF!</v>
+        <v>8333.2240000000002</v>
       </c>
     </row>
   </sheetData>
@@ -5084,15 +5301,39 @@
     <hyperlink ref="G13" r:id="rId18"/>
     <hyperlink ref="G14" r:id="rId19"/>
     <hyperlink ref="J14" r:id="rId20"/>
-    <hyperlink ref="G15" r:id="rId21"/>
-    <hyperlink ref="G16" r:id="rId22"/>
-    <hyperlink ref="G18" r:id="rId23"/>
-    <hyperlink ref="G20" r:id="rId24"/>
-    <hyperlink ref="G21" r:id="rId25"/>
-    <hyperlink ref="G22" r:id="rId26"/>
-    <hyperlink ref="G24" r:id="rId27"/>
+    <hyperlink ref="G16" r:id="rId21"/>
+    <hyperlink ref="G18" r:id="rId22"/>
+    <hyperlink ref="G20" r:id="rId23"/>
+    <hyperlink ref="G21" r:id="rId24"/>
+    <hyperlink ref="G22" r:id="rId25"/>
+    <hyperlink ref="G24" r:id="rId26"/>
+    <hyperlink ref="G40" r:id="rId27"/>
+    <hyperlink ref="G44" r:id="rId28"/>
+    <hyperlink ref="G45" r:id="rId29"/>
+    <hyperlink ref="G47" r:id="rId30"/>
+    <hyperlink ref="G51" r:id="rId31"/>
+    <hyperlink ref="G52" r:id="rId32"/>
+    <hyperlink ref="G60" r:id="rId33"/>
+    <hyperlink ref="G62" r:id="rId34"/>
+    <hyperlink ref="G63" r:id="rId35"/>
+    <hyperlink ref="G64" r:id="rId36"/>
+    <hyperlink ref="G65" r:id="rId37"/>
+    <hyperlink ref="G66" r:id="rId38"/>
+    <hyperlink ref="G67" r:id="rId39"/>
+    <hyperlink ref="G68" r:id="rId40"/>
+    <hyperlink ref="G70" r:id="rId41"/>
+    <hyperlink ref="G71" r:id="rId42"/>
+    <hyperlink ref="J76" r:id="rId43"/>
+    <hyperlink ref="J78" r:id="rId44"/>
+    <hyperlink ref="J79" r:id="rId45"/>
+    <hyperlink ref="J80" r:id="rId46"/>
+    <hyperlink ref="J81" r:id="rId47"/>
+    <hyperlink ref="G84" r:id="rId48"/>
+    <hyperlink ref="J86" r:id="rId49"/>
+    <hyperlink ref="J74" r:id="rId50"/>
+    <hyperlink ref="G74" r:id="rId51"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId52"/>
 </worksheet>
 </file>
</xml_diff>